<commit_message>
remove unreliable data from input data file
</commit_message>
<xml_diff>
--- a/all_tests.xlsx
+++ b/all_tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="MBC" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,8 +18,9 @@
     <sheet name="NO3" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="AS" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="TOC" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="EC" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="qCO2" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="TON" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="EC" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="qCO2" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="10">
   <si>
     <t xml:space="preserve">MIN</t>
   </si>
@@ -75,12 +76,13 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -97,132 +99,13 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="13">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -249,27 +132,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -287,7 +155,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,76 +179,25 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -388,11 +205,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -400,43 +217,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,7 +277,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -472,7 +289,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -481,57 +298,40 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -547,7 +347,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -579,7 +379,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="R20" activeCellId="1" sqref="S14:W21 R20"/>
+      <selection pane="topRight" activeCell="R20" activeCellId="0" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1493,8 +1293,8 @@
   </sheetPr>
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="1" sqref="S14:W21 R1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1890,8 +1690,291 @@
   </sheetPr>
   <dimension ref="A1:Y5"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="T3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="U3" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="V3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="X3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.087787389755249</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.101020343601704</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.097668468952179</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.0911238938570023</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.150896772742271</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.141061395406723</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.169345259666443</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.132711112499237</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>0.11294137686491</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.106409326195717</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0.108985930681229</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.0930154472589493</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.0849529728293419</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.0948345810174942</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.0855105444788933</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.15741916000843</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.152956768870354</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.161884903907776</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.164237901568413</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.111144565045834</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.0950553640723228</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.0999634638428688</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.0912019610404968</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0.105798281729221</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0.0897916778922081</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.0845823511481285</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0.155468106269836</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0.162625223398209</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>0.173704087734222</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.118197947740555</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>0.112112283706665</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>0.116324782371521</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Y5"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="S14:W21 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2206,7 +2289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2214,7 +2297,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="S14:W21 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2297,7 +2380,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A6" activeCellId="1" sqref="S14:W21 A6"/>
+      <selection pane="topRight" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2861,7 +2944,7 @@
   <dimension ref="A1:AA15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="1" sqref="S14:W21 A16"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3425,7 +3508,7 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S14:W21 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3989,7 +4072,7 @@
   <dimension ref="A1:Y8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V8" activeCellId="1" sqref="S14:W21 V8"/>
+      <selection pane="topLeft" activeCell="V8" activeCellId="0" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4542,12 +4625,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="W14" activeCellId="0" sqref="S14:W21"/>
+      <selection pane="topRight" activeCell="W14" activeCellId="0" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5407,7 +5490,7 @@
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="1" sqref="S14:W21 A15"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5800,7 +5883,7 @@
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="1" sqref="S14:W21 F21"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6185,8 +6268,8 @@
   </sheetPr>
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S14:W21 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>